<commit_message>
Completed bench grinder risk assessment
</commit_message>
<xml_diff>
--- a/Health & Safety/Risk Assessments/Risk Assessment - Bench Grinder.xlsx
+++ b/Health & Safety/Risk Assessments/Risk Assessment - Bench Grinder.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="3D Printing" sheetId="1" r:id="rId1"/>
+    <sheet name="Bench Grinder" sheetId="1" r:id="rId1"/>
     <sheet name="Risk Assessment Guide" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725" refMode="R1C1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
   <si>
     <t>Hazard to health and/or safety present</t>
   </si>
@@ -128,14 +128,65 @@
     <t>Action Within 12 Months</t>
   </si>
   <si>
-    <t>TO BE COMPLETED!</t>
+    <t>Sparks</t>
+  </si>
+  <si>
+    <t>Getting caught in mechanism</t>
+  </si>
+  <si>
+    <t>Could cause ignition, small burns or blind</t>
+  </si>
+  <si>
+    <t>Abrasion against skin from wheel</t>
+  </si>
+  <si>
+    <t>Entanglement could pose a fire escape risk, cause abrasions, force hard contact and removal hair and scalp.</t>
+  </si>
+  <si>
+    <t>Could cause friction burns, remove skin and flesh</t>
+  </si>
+  <si>
+    <t>Explosion from wheel being jammed</t>
+  </si>
+  <si>
+    <t>Explosion from unbalanced wheels - Wheels could explode if they become unbalanced.  This can occur from misuse of the machine such as grinding non ferrous metals or plastics.</t>
+  </si>
+  <si>
+    <t>Explosion from mixture of materials- Some materials (for example iron and aluminium) could create a chemical reaction if mixed heat added from the grinding process.</t>
+  </si>
+  <si>
+    <t>Parts of workpiece breaking up</t>
+  </si>
+  <si>
+    <t>Parts of workpiece being sent flying</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> An exposion of a grinding wheel could cause debris to injur or possible kill the operator or anybody nearby.  The heat of the explosion could also cause burn and pose a fire risk.</t>
+  </si>
+  <si>
+    <t>Parts of the workpiece could chip off and become flying debris.  This could injur or blind the operator or those nearby</t>
+  </si>
+  <si>
+    <t>The entire workpiece could be sent flying at dangerous speeds.  This could injur or blind the operator or those nearby.  If the piece is sharp (i.e. a chisel) then it could also pentrate the body.</t>
+  </si>
+  <si>
+    <t>Circulate risk assessment, create basic training, print and display warning poster and ensure in place before 31.12.15</t>
+  </si>
+  <si>
+    <t>Rule exists that nobody may use the equipment on their own or if not a member.  Also rules state that you may not use the tool unless you are confident and qualified to do so.</t>
+  </si>
+  <si>
+    <t>Rule exists that nobody may use the equipment on their own or if not a member.  Also rules state that you may not use the tool unless you are confident and qualified to do so.  The machine has a guard to prevent sparks from flying at the operators face and PPE including goggles are provided.</t>
+  </si>
+  <si>
+    <t>Rule exists that nobody may use the equipment on their own or if not a member.  Also rules state that you may not use the tool unless you are confident and qualified to do so.  The machine has a guard to prevent parts from flying at the operators face and PPE including goggles are provided.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,8 +258,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="48"/>
-      <color rgb="FFFF0000"/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -240,7 +290,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -461,40 +511,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -560,32 +582,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -608,12 +609,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,6 +718,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -740,6 +753,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -915,290 +929,425 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" customWidth="1"/>
-    <col min="5" max="5" width="40.85546875" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" style="43" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" style="43" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" style="43" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="43" customWidth="1"/>
+    <col min="5" max="5" width="40.85546875" style="43" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.5">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="50" t="s">
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+    </row>
+    <row r="2" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="51"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="51"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="51"/>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="51"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="40"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="40"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="40"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="40"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="40"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="41"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="41"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="41"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="C15" s="1"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="41"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="41"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="41"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="41"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="41"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
+      <c r="B5" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="44"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="44"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="44"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="45"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="45"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="45"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="45"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="45"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="45"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="45"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="45"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="45"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="45"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="45"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="45"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="45"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="45"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="45"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="47"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="47"/>
+      <c r="B35" s="47"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="47"/>
+      <c r="B36" s="47"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="47"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="47"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="47"/>
+      <c r="B39" s="47"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="47"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="47"/>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="47"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="47"/>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="47"/>
+      <c r="B42" s="47"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:E6"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61.140625" customWidth="1"/>
@@ -1210,147 +1359,147 @@
     <col min="9" max="9" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29.25" thickBot="1">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="49"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="18" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="40"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="24" thickBot="1">
-      <c r="A2" s="43" t="s">
+    <row r="2" spans="1:9" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="45" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="F2" s="21" t="s">
+      <c r="D2" s="37"/>
+      <c r="F2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18.75">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18.75">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18.75">
-      <c r="F6" s="25" t="s">
+    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F6" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:9" ht="18.75">
-      <c r="F7" s="27" t="s">
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F7" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="16"/>
-    </row>
-    <row r="8" spans="1:9" ht="18.75">
-      <c r="F8" s="29" t="s">
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F8" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="H8" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="17"/>
+      <c r="I8" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>